<commit_message>
major refactoring and add operation example
</commit_message>
<xml_diff>
--- a/docs/template-basic.xlsx
+++ b/docs/template-basic.xlsx
@@ -331,7 +331,7 @@
     <t>Simple_Extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://www.fhir.org/guides/ig-sampler/StructureDefinition/extension-blah}
+    <t xml:space="preserve">Extension {http://www.fhir.org/guides/sampler2/StructureDefinition/extension-blah}
 </t>
   </si>
   <si>
@@ -352,7 +352,7 @@
     <t>Complex_Extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://www.fhir.org/guides/ig-sampler/StructureDefinition/extension-complex}
+    <t xml:space="preserve">Extension {http://www.fhir.org/guides/sampler2/StructureDefinition/extension-complex}
 </t>
   </si>
   <si>

</xml_diff>